<commit_message>
Carga y actualiza subtareas
</commit_message>
<xml_diff>
--- a/Plan/Proyectos Operaciones DCTI 2018(SCRUM).xlsx
+++ b/Plan/Proyectos Operaciones DCTI 2018(SCRUM).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalCDC\Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG + STORIES" sheetId="2" r:id="rId1"/>
@@ -1056,57 +1056,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="14" borderId="12" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="16" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="15" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="14" borderId="15" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="10" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1118,6 +1067,57 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="16" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="15" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="14" borderId="12" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="14" borderId="15" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1940,7 +1940,7 @@
                     <c:v>28</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>4</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1964,7 +1964,7 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,61 +2221,61 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2847,7 +2847,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.3333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -6105,9 +6105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6148,16 +6148,16 @@
       <c r="H1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="74"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="93">
+      <c r="B2" s="76">
         <v>13</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -6174,7 +6174,7 @@
       </c>
       <c r="G2" s="71">
         <f>VLOOKUP(B2,'SPRINT Points'!$A$4:$E$99,5,FALSE)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="27" t="s">
         <v>52</v>
@@ -6190,7 +6190,7 @@
       <c r="A3" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="93">
+      <c r="B3" s="76">
         <v>14</v>
       </c>
       <c r="C3" s="35" t="s">
@@ -6207,7 +6207,7 @@
       </c>
       <c r="G3" s="71">
         <f>VLOOKUP(B3,'SPRINT Points'!$A$4:$E$99,5,FALSE)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>55</v>
@@ -6223,7 +6223,7 @@
       <c r="A4" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="93">
+      <c r="B4" s="76">
         <v>18</v>
       </c>
       <c r="C4" s="35" t="s">
@@ -6256,7 +6256,7 @@
       <c r="A5" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="93">
+      <c r="B5" s="76">
         <v>15</v>
       </c>
       <c r="C5" s="36" t="s">
@@ -6283,7 +6283,7 @@
       <c r="A6" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="93">
+      <c r="B6" s="76">
         <v>16</v>
       </c>
       <c r="C6" s="35" t="s">
@@ -6305,10 +6305,10 @@
       <c r="H6" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="75"/>
+      <c r="K6" s="79"/>
       <c r="L6" s="32" t="s">
         <v>34</v>
       </c>
@@ -6317,7 +6317,7 @@
       <c r="A7" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="93">
+      <c r="B7" s="76">
         <v>17</v>
       </c>
       <c r="C7" s="35" t="s">
@@ -6352,7 +6352,7 @@
       <c r="A8" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="93">
+      <c r="B8" s="76">
         <v>11</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -6387,7 +6387,7 @@
       <c r="A9" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="93">
+      <c r="B9" s="76">
         <v>12</v>
       </c>
       <c r="C9" s="35" t="s">
@@ -6422,7 +6422,7 @@
       <c r="A10" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="93">
+      <c r="B10" s="76">
         <v>19</v>
       </c>
       <c r="C10" s="35" t="s">
@@ -6457,7 +6457,7 @@
       <c r="A11" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="93">
+      <c r="B11" s="76">
         <v>20</v>
       </c>
       <c r="C11" s="35" t="s">
@@ -6484,7 +6484,7 @@
       <c r="A12" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="93">
+      <c r="B12" s="76">
         <v>21</v>
       </c>
       <c r="C12" s="35" t="s">
@@ -6508,7 +6508,7 @@
       <c r="A13" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="93">
+      <c r="B13" s="76">
         <v>22</v>
       </c>
       <c r="C13" s="35" t="s">
@@ -6530,703 +6530,703 @@
     </row>
     <row r="14" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="40"/>
-      <c r="B14" s="93"/>
+      <c r="B14" s="76"/>
       <c r="G14" s="71"/>
     </row>
     <row r="15" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
-      <c r="B15" s="93"/>
+      <c r="B15" s="76"/>
       <c r="G15" s="71"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="40"/>
-      <c r="B16" s="93"/>
+      <c r="B16" s="76"/>
       <c r="C16" s="20"/>
       <c r="G16" s="71"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
-      <c r="B17" s="93"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="36"/>
       <c r="D17" s="68"/>
       <c r="G17" s="71"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="40"/>
-      <c r="B18" s="93"/>
+      <c r="B18" s="76"/>
       <c r="G18" s="71"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="40"/>
-      <c r="B19" s="93"/>
+      <c r="B19" s="76"/>
       <c r="G19" s="71"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="40"/>
-      <c r="B20" s="93"/>
+      <c r="B20" s="76"/>
       <c r="G20" s="71"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
-      <c r="B21" s="93"/>
+      <c r="B21" s="76"/>
       <c r="G21" s="71"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
-      <c r="B22" s="93"/>
+      <c r="B22" s="76"/>
       <c r="G22" s="71"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
-      <c r="B23" s="93"/>
+      <c r="B23" s="76"/>
       <c r="G23" s="71"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
-      <c r="B24" s="93"/>
+      <c r="B24" s="76"/>
       <c r="G24" s="71"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
-      <c r="B25" s="93"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="36"/>
       <c r="G25" s="71"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
-      <c r="B26" s="93"/>
+      <c r="B26" s="76"/>
       <c r="G26" s="71"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
-      <c r="B27" s="93"/>
+      <c r="B27" s="76"/>
       <c r="G27" s="71"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
-      <c r="B28" s="90"/>
+      <c r="B28" s="73"/>
       <c r="G28" s="71"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
-      <c r="B29" s="90"/>
+      <c r="B29" s="73"/>
       <c r="G29" s="71"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
-      <c r="B30" s="90"/>
+      <c r="B30" s="73"/>
       <c r="G30" s="71"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
-      <c r="B31" s="90"/>
+      <c r="B31" s="73"/>
       <c r="G31" s="71"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
-      <c r="B32" s="90"/>
+      <c r="B32" s="73"/>
       <c r="G32" s="71"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
-      <c r="B33" s="90"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="20"/>
       <c r="G33" s="71"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
-      <c r="B34" s="90"/>
+      <c r="B34" s="73"/>
       <c r="G34" s="71"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
-      <c r="B35" s="90"/>
+      <c r="B35" s="73"/>
       <c r="G35" s="71"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="40"/>
-      <c r="B36" s="90"/>
+      <c r="B36" s="73"/>
       <c r="G36" s="71"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="90"/>
+      <c r="B37" s="73"/>
       <c r="G37" s="71"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
-      <c r="B38" s="90"/>
+      <c r="B38" s="73"/>
       <c r="G38" s="71"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
-      <c r="B39" s="90"/>
+      <c r="B39" s="73"/>
       <c r="G39" s="71"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
-      <c r="B40" s="90"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="36"/>
       <c r="G40" s="71"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
-      <c r="B41" s="90"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="31"/>
       <c r="G41" s="71"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
-      <c r="B42" s="90"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="36"/>
       <c r="G42" s="71"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
-      <c r="B43" s="90"/>
+      <c r="B43" s="73"/>
       <c r="G43" s="71"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
-      <c r="B44" s="90"/>
+      <c r="B44" s="73"/>
       <c r="G44" s="71"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
-      <c r="B45" s="90"/>
+      <c r="B45" s="73"/>
       <c r="G45" s="71"/>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
-      <c r="B46" s="90"/>
+      <c r="B46" s="73"/>
       <c r="G46" s="71"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
-      <c r="B47" s="90"/>
+      <c r="B47" s="73"/>
       <c r="G47" s="71"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="90"/>
+      <c r="B48" s="73"/>
       <c r="G48" s="71"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="91"/>
+      <c r="B49" s="74"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="91"/>
+      <c r="B50" s="74"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="91"/>
+      <c r="B51" s="74"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="91"/>
+      <c r="B52" s="74"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="91"/>
+      <c r="B53" s="74"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" s="91"/>
+      <c r="B54" s="74"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="91"/>
+      <c r="B55" s="74"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56" s="91"/>
+      <c r="B56" s="74"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="91"/>
+      <c r="B57" s="74"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="91"/>
+      <c r="B58" s="74"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B59" s="91"/>
+      <c r="B59" s="74"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B60" s="91"/>
+      <c r="B60" s="74"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B61" s="91"/>
+      <c r="B61" s="74"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B62" s="91"/>
+      <c r="B62" s="74"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B63" s="91"/>
+      <c r="B63" s="74"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B64" s="91"/>
+      <c r="B64" s="74"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B65" s="91"/>
+      <c r="B65" s="74"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B66" s="91"/>
+      <c r="B66" s="74"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B67" s="91"/>
+      <c r="B67" s="74"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B68" s="91"/>
+      <c r="B68" s="74"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B69" s="91"/>
+      <c r="B69" s="74"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B70" s="91"/>
+      <c r="B70" s="74"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B71" s="91"/>
+      <c r="B71" s="74"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B72" s="91"/>
+      <c r="B72" s="74"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B73" s="91"/>
+      <c r="B73" s="74"/>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B74" s="91"/>
+      <c r="B74" s="74"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B75" s="91"/>
+      <c r="B75" s="74"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B76" s="91"/>
+      <c r="B76" s="74"/>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B77" s="91"/>
+      <c r="B77" s="74"/>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B78" s="91"/>
+      <c r="B78" s="74"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B79" s="91"/>
+      <c r="B79" s="74"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B80" s="91"/>
+      <c r="B80" s="74"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" s="91"/>
+      <c r="B81" s="74"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B82" s="91"/>
+      <c r="B82" s="74"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B83" s="91"/>
+      <c r="B83" s="74"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B84" s="91"/>
+      <c r="B84" s="74"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B85" s="91"/>
+      <c r="B85" s="74"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B86" s="91"/>
+      <c r="B86" s="74"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B87" s="91"/>
+      <c r="B87" s="74"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B88" s="91"/>
+      <c r="B88" s="74"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B89" s="91"/>
+      <c r="B89" s="74"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B90" s="91"/>
+      <c r="B90" s="74"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B91" s="91"/>
+      <c r="B91" s="74"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B92" s="91"/>
+      <c r="B92" s="74"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B93" s="91"/>
+      <c r="B93" s="74"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B94" s="91"/>
+      <c r="B94" s="74"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B95" s="91"/>
+      <c r="B95" s="74"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B96" s="91"/>
+      <c r="B96" s="74"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B97" s="91"/>
+      <c r="B97" s="74"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B98" s="91"/>
+      <c r="B98" s="74"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B99" s="91"/>
+      <c r="B99" s="74"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B100" s="91"/>
+      <c r="B100" s="74"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B101" s="91"/>
+      <c r="B101" s="74"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B102" s="91"/>
+      <c r="B102" s="74"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B103" s="91"/>
+      <c r="B103" s="74"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B104" s="91"/>
+      <c r="B104" s="74"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B105" s="91"/>
+      <c r="B105" s="74"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B106" s="91"/>
+      <c r="B106" s="74"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B107" s="91"/>
+      <c r="B107" s="74"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B108" s="91"/>
+      <c r="B108" s="74"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B109" s="91"/>
+      <c r="B109" s="74"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B110" s="91"/>
+      <c r="B110" s="74"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B111" s="91"/>
+      <c r="B111" s="74"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B112" s="91"/>
+      <c r="B112" s="74"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B113" s="91"/>
+      <c r="B113" s="74"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B114" s="91"/>
+      <c r="B114" s="74"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B115" s="91"/>
+      <c r="B115" s="74"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B116" s="91"/>
+      <c r="B116" s="74"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B117" s="91"/>
+      <c r="B117" s="74"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B118" s="91"/>
+      <c r="B118" s="74"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B119" s="91"/>
+      <c r="B119" s="74"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B120" s="91"/>
+      <c r="B120" s="74"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B121" s="91"/>
+      <c r="B121" s="74"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B122" s="91"/>
+      <c r="B122" s="74"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B123" s="91"/>
+      <c r="B123" s="74"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B124" s="91"/>
+      <c r="B124" s="74"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B125" s="91"/>
+      <c r="B125" s="74"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B126" s="91"/>
+      <c r="B126" s="74"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B127" s="91"/>
+      <c r="B127" s="74"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B128" s="91"/>
+      <c r="B128" s="74"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B129" s="91"/>
+      <c r="B129" s="74"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B130" s="91"/>
+      <c r="B130" s="74"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B131" s="91"/>
+      <c r="B131" s="74"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B132" s="91"/>
+      <c r="B132" s="74"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B133" s="91"/>
+      <c r="B133" s="74"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B134" s="91"/>
+      <c r="B134" s="74"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B135" s="91"/>
+      <c r="B135" s="74"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B136" s="91"/>
+      <c r="B136" s="74"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B137" s="91"/>
+      <c r="B137" s="74"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B138" s="91"/>
+      <c r="B138" s="74"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B139" s="91"/>
+      <c r="B139" s="74"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B140" s="91"/>
+      <c r="B140" s="74"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B141" s="91"/>
+      <c r="B141" s="74"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B142" s="91"/>
+      <c r="B142" s="74"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B143" s="91"/>
+      <c r="B143" s="74"/>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B144" s="91"/>
+      <c r="B144" s="74"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B145" s="91"/>
+      <c r="B145" s="74"/>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B146" s="91"/>
+      <c r="B146" s="74"/>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B147" s="91"/>
+      <c r="B147" s="74"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B148" s="91"/>
+      <c r="B148" s="74"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B149" s="91"/>
+      <c r="B149" s="74"/>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B150" s="91"/>
+      <c r="B150" s="74"/>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B151" s="91"/>
+      <c r="B151" s="74"/>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B152" s="91"/>
+      <c r="B152" s="74"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B153" s="91"/>
+      <c r="B153" s="74"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B154" s="91"/>
+      <c r="B154" s="74"/>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B155" s="91"/>
+      <c r="B155" s="74"/>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B156" s="91"/>
+      <c r="B156" s="74"/>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B157" s="91"/>
+      <c r="B157" s="74"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B158" s="91"/>
+      <c r="B158" s="74"/>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B159" s="91"/>
+      <c r="B159" s="74"/>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B160" s="91"/>
+      <c r="B160" s="74"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B161" s="91"/>
+      <c r="B161" s="74"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B162" s="91"/>
+      <c r="B162" s="74"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B163" s="91"/>
+      <c r="B163" s="74"/>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B164" s="91"/>
+      <c r="B164" s="74"/>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B165" s="91"/>
+      <c r="B165" s="74"/>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B166" s="91"/>
+      <c r="B166" s="74"/>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B167" s="91"/>
+      <c r="B167" s="74"/>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B168" s="91"/>
+      <c r="B168" s="74"/>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B169" s="91"/>
+      <c r="B169" s="74"/>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B170" s="91"/>
+      <c r="B170" s="74"/>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B171" s="91"/>
+      <c r="B171" s="74"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B172" s="91"/>
+      <c r="B172" s="74"/>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B173" s="91"/>
+      <c r="B173" s="74"/>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B174" s="91"/>
+      <c r="B174" s="74"/>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B175" s="91"/>
+      <c r="B175" s="74"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B176" s="91"/>
+      <c r="B176" s="74"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B177" s="91"/>
+      <c r="B177" s="74"/>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B178" s="91"/>
+      <c r="B178" s="74"/>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B179" s="91"/>
+      <c r="B179" s="74"/>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B180" s="91"/>
+      <c r="B180" s="74"/>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B181" s="91"/>
+      <c r="B181" s="74"/>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B182" s="91"/>
+      <c r="B182" s="74"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B183" s="91"/>
+      <c r="B183" s="74"/>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B184" s="91"/>
+      <c r="B184" s="74"/>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B185" s="91"/>
+      <c r="B185" s="74"/>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B186" s="91"/>
+      <c r="B186" s="74"/>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B187" s="91"/>
+      <c r="B187" s="74"/>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B188" s="91"/>
+      <c r="B188" s="74"/>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B189" s="91"/>
+      <c r="B189" s="74"/>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B190" s="91"/>
+      <c r="B190" s="74"/>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B191" s="91"/>
+      <c r="B191" s="74"/>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B192" s="91"/>
+      <c r="B192" s="74"/>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B193" s="91"/>
+      <c r="B193" s="74"/>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B194" s="91"/>
+      <c r="B194" s="74"/>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B195" s="91"/>
+      <c r="B195" s="74"/>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B196" s="91"/>
+      <c r="B196" s="74"/>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B197" s="91"/>
+      <c r="B197" s="74"/>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B198" s="91"/>
+      <c r="B198" s="74"/>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B199" s="91"/>
+      <c r="B199" s="74"/>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B200" s="91"/>
+      <c r="B200" s="74"/>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B201" s="91"/>
+      <c r="B201" s="74"/>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B202" s="91"/>
+      <c r="B202" s="74"/>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B203" s="91"/>
+      <c r="B203" s="74"/>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B204" s="91"/>
+      <c r="B204" s="74"/>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B205" s="91"/>
+      <c r="B205" s="74"/>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B206" s="91"/>
+      <c r="B206" s="74"/>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B207" s="91"/>
+      <c r="B207" s="74"/>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B208" s="91"/>
+      <c r="B208" s="74"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B209" s="91"/>
+      <c r="B209" s="74"/>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B210" s="91"/>
+      <c r="B210" s="74"/>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B211" s="91"/>
+      <c r="B211" s="74"/>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B212" s="91"/>
+      <c r="B212" s="74"/>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B213" s="91"/>
+      <c r="B213" s="74"/>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B214" s="91"/>
+      <c r="B214" s="74"/>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B215" s="91"/>
+      <c r="B215" s="74"/>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B216" s="91"/>
+      <c r="B216" s="74"/>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B217" s="91"/>
+      <c r="B217" s="74"/>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B218" s="91"/>
+      <c r="B218" s="74"/>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B219" s="91"/>
+      <c r="B219" s="74"/>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B220" s="91"/>
+      <c r="B220" s="74"/>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B221" s="91"/>
+      <c r="B221" s="74"/>
     </row>
   </sheetData>
   <sortState ref="A2:H48">
@@ -7268,7 +7268,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7300,77 +7300,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="86"/>
+      <c r="H1" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="84" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="84"/>
-      <c r="N1" s="82" t="s">
+      <c r="M1" s="86"/>
+      <c r="N1" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="83" t="s">
+      <c r="O1" s="87"/>
+      <c r="P1" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="84" t="s">
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="84"/>
-      <c r="T1" s="82" t="s">
+      <c r="S1" s="86"/>
+      <c r="T1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="82"/>
-      <c r="V1" s="83" t="s">
+      <c r="U1" s="87"/>
+      <c r="V1" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="83"/>
-      <c r="X1" s="84" t="s">
+      <c r="W1" s="85"/>
+      <c r="X1" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="82" t="s">
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="83" t="s">
+      <c r="AA1" s="87"/>
+      <c r="AB1" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="83"/>
+      <c r="AC1" s="85"/>
       <c r="AD1" s="43"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="50">
         <v>1</v>
       </c>
@@ -7475,7 +7475,7 @@
       <c r="AC3" s="46"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="92">
+      <c r="A4" s="75">
         <v>13</v>
       </c>
       <c r="B4" s="26" t="str">
@@ -7491,14 +7491,16 @@
       </c>
       <c r="E4" s="6">
         <f t="shared" ref="E4:E22" si="1">IF(D4&gt;C4,$D4-(SUM($F4:$AC4)),$C4-(SUM($F4:$AC4)))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="52"/>
       <c r="G4" s="53"/>
       <c r="H4" s="60"/>
       <c r="I4" s="59"/>
       <c r="J4" s="47"/>
-      <c r="K4" s="63"/>
+      <c r="K4" s="63">
+        <v>2</v>
+      </c>
       <c r="L4" s="53"/>
       <c r="M4" s="53"/>
       <c r="N4" s="60"/>
@@ -7519,7 +7521,7 @@
       <c r="AC4" s="47"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="92">
+      <c r="A5" s="75">
         <v>14</v>
       </c>
       <c r="B5" s="26" t="str">
@@ -7535,14 +7537,16 @@
       </c>
       <c r="E5" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" s="54"/>
       <c r="G5" s="50"/>
       <c r="H5" s="59"/>
       <c r="I5" s="59"/>
       <c r="J5" s="48"/>
-      <c r="K5" s="64"/>
+      <c r="K5" s="64">
+        <v>2</v>
+      </c>
       <c r="L5" s="55"/>
       <c r="M5" s="50"/>
       <c r="N5" s="59"/>
@@ -7563,7 +7567,7 @@
       <c r="AC5" s="45"/>
     </row>
     <row r="6" spans="1:30" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92">
+      <c r="A6" s="75">
         <v>18</v>
       </c>
       <c r="B6" s="26" t="str">
@@ -7607,7 +7611,7 @@
       <c r="AC6" s="45"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="92"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="26" t="str">
         <f>IF(A7="","", VLOOKUP(A7,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A7,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A7,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7647,7 +7651,7 @@
       <c r="AC7" s="45"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="26" t="str">
         <f>IF(A8="","", VLOOKUP(A8,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A8,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A8,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7687,7 +7691,7 @@
       <c r="AC8" s="45"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="26" t="str">
         <f>IF(A9="","", VLOOKUP(A9,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A9,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A9,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7727,7 +7731,7 @@
       <c r="AC9" s="45"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="26" t="str">
         <f>IF(A10="","", VLOOKUP(A10,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A10,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A10,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7767,7 +7771,7 @@
       <c r="AC10" s="45"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="26" t="str">
         <f>IF(A11="","", VLOOKUP(A11,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A11,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A11,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7807,7 +7811,7 @@
       <c r="AC11" s="45"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="26" t="str">
         <f>IF(A12="","", VLOOKUP(A12,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A12,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A12,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7847,7 +7851,7 @@
       <c r="AC12" s="45"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
+      <c r="A13" s="75"/>
       <c r="B13" s="26" t="str">
         <f>IF(A13="","", VLOOKUP(A13,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A13,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A13,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7887,7 +7891,7 @@
       <c r="AC13" s="45"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="92"/>
+      <c r="A14" s="75"/>
       <c r="B14" s="26" t="str">
         <f>IF(A14="","", VLOOKUP(A14,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A14,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A14,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7927,7 +7931,7 @@
       <c r="AC14" s="45"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="26" t="str">
         <f>IF(A15="","", VLOOKUP(A15,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A15,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A15,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -7967,7 +7971,7 @@
       <c r="AC15" s="45"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="26" t="str">
         <f>IF(A16="","", VLOOKUP(A16,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A16,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A16,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8007,7 +8011,7 @@
       <c r="AC16" s="45"/>
     </row>
     <row r="17" spans="1:29" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="26" t="str">
         <f>IF(A17="","", VLOOKUP(A17,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A17,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A17,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8047,7 +8051,7 @@
       <c r="AC17" s="45"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
+      <c r="A18" s="75"/>
       <c r="B18" s="26" t="str">
         <f>IF(A18="","", VLOOKUP(A18,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A18,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A18,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8087,7 +8091,7 @@
       <c r="AC18" s="45"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="92"/>
+      <c r="A19" s="75"/>
       <c r="B19" s="26" t="str">
         <f>IF(A19="","", VLOOKUP(A19,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A19,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A19,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8127,7 +8131,7 @@
       <c r="AC19" s="45"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
+      <c r="A20" s="75"/>
       <c r="B20" s="26" t="str">
         <f>IF(A20="","", VLOOKUP(A20,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A20,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A20,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8167,7 +8171,7 @@
       <c r="AC20" s="45"/>
     </row>
     <row r="21" spans="1:29" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="26" t="str">
         <f>IF(A21="","", VLOOKUP(A21,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A21,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A21,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8207,7 +8211,7 @@
       <c r="AC21" s="45"/>
     </row>
     <row r="22" spans="1:29" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
+      <c r="A22" s="75"/>
       <c r="B22" s="26" t="str">
         <f>IF(A22="","", VLOOKUP(A22,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A22,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A22,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8247,7 +8251,7 @@
       <c r="AC22" s="45"/>
     </row>
     <row r="23" spans="1:29" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="92"/>
+      <c r="A23" s="75"/>
       <c r="B23" s="26" t="str">
         <f>IF(A23="","", VLOOKUP(A23,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A23,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A23,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8287,7 +8291,7 @@
       <c r="AC23" s="45"/>
     </row>
     <row r="24" spans="1:29" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
+      <c r="A24" s="75"/>
       <c r="B24" s="26" t="str">
         <f>IF(A24="","", VLOOKUP(A24,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A24,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A24,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8327,7 +8331,7 @@
       <c r="AC24" s="45"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
+      <c r="A25" s="75"/>
       <c r="B25" s="26" t="str">
         <f>IF(A25="","", VLOOKUP(A25,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A25,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A25,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8361,7 +8365,7 @@
       <c r="AC25" s="45"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
+      <c r="A26" s="75"/>
       <c r="B26" s="26" t="str">
         <f>IF(A26="","", VLOOKUP(A26,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A26,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A26,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8395,7 +8399,7 @@
       <c r="AC26" s="45"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="26" t="str">
         <f>IF(A27="","", VLOOKUP(A27,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A27,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A27,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8429,7 +8433,7 @@
       <c r="AC27" s="45"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
+      <c r="A28" s="75"/>
       <c r="B28" s="26" t="str">
         <f>IF(A28="","", VLOOKUP(A28,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A28,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A28,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8463,7 +8467,7 @@
       <c r="AC28" s="45"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="92"/>
+      <c r="A29" s="75"/>
       <c r="B29" s="26" t="str">
         <f>IF(A29="","", VLOOKUP(A29,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A29,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A29,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -8497,7 +8501,7 @@
       <c r="AC29" s="45"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
+      <c r="A30" s="75"/>
       <c r="B30" s="26" t="str">
         <f>IF(A30="","", VLOOKUP(A30,'BACKLOG + STORIES'!$B$1:$F$181,3,FALSE) &amp; " (" &amp; VLOOKUP(A30,'BACKLOG + STORIES'!$B$1:$F$181,4,FALSE) &amp; VLOOKUP(A30,'BACKLOG + STORIES'!$B$1:$F$181,5,FALSE)&amp; ")" )</f>
         <v/>
@@ -10896,7 +10900,7 @@
       </c>
       <c r="E100" s="45">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F100" s="56">
         <f t="shared" si="4"/>
@@ -10920,7 +10924,7 @@
       </c>
       <c r="K100" s="65">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L100" s="56">
         <f t="shared" si="4"/>
@@ -11005,32 +11009,32 @@
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="12"/>
-      <c r="F101" s="81"/>
-      <c r="G101" s="79"/>
-      <c r="H101" s="80"/>
-      <c r="I101" s="80"/>
-      <c r="J101" s="77">
+      <c r="F101" s="93"/>
+      <c r="G101" s="81"/>
+      <c r="H101" s="91"/>
+      <c r="I101" s="91"/>
+      <c r="J101" s="89">
         <v>28</v>
       </c>
-      <c r="K101" s="78"/>
-      <c r="L101" s="79"/>
-      <c r="M101" s="79"/>
-      <c r="N101" s="80"/>
-      <c r="O101" s="80"/>
-      <c r="P101" s="77"/>
-      <c r="Q101" s="78"/>
-      <c r="R101" s="79"/>
-      <c r="S101" s="79"/>
-      <c r="T101" s="80"/>
-      <c r="U101" s="80"/>
-      <c r="V101" s="77"/>
-      <c r="W101" s="78"/>
-      <c r="X101" s="79"/>
-      <c r="Y101" s="79"/>
-      <c r="Z101" s="80"/>
-      <c r="AA101" s="80"/>
-      <c r="AB101" s="77"/>
-      <c r="AC101" s="77"/>
+      <c r="K101" s="90"/>
+      <c r="L101" s="81"/>
+      <c r="M101" s="81"/>
+      <c r="N101" s="91"/>
+      <c r="O101" s="91"/>
+      <c r="P101" s="89"/>
+      <c r="Q101" s="90"/>
+      <c r="R101" s="81"/>
+      <c r="S101" s="81"/>
+      <c r="T101" s="91"/>
+      <c r="U101" s="91"/>
+      <c r="V101" s="89"/>
+      <c r="W101" s="90"/>
+      <c r="X101" s="81"/>
+      <c r="Y101" s="81"/>
+      <c r="Z101" s="91"/>
+      <c r="AA101" s="91"/>
+      <c r="AB101" s="89"/>
+      <c r="AC101" s="89"/>
     </row>
     <row r="102" spans="1:29" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B102" s="29" t="s">
@@ -11044,81 +11048,81 @@
         <f>C100</f>
         <v>28</v>
       </c>
-      <c r="F102" s="79">
+      <c r="F102" s="81">
         <f>E102-F101</f>
         <v>28</v>
       </c>
-      <c r="G102" s="79"/>
-      <c r="H102" s="80">
+      <c r="G102" s="81"/>
+      <c r="H102" s="91">
         <f>F102-H101</f>
         <v>28</v>
       </c>
-      <c r="I102" s="80"/>
-      <c r="J102" s="77">
+      <c r="I102" s="91"/>
+      <c r="J102" s="89">
         <f>H102-J101</f>
         <v>0</v>
       </c>
-      <c r="K102" s="78"/>
-      <c r="L102" s="79">
+      <c r="K102" s="90"/>
+      <c r="L102" s="81">
         <f>J102-L101</f>
         <v>0</v>
       </c>
-      <c r="M102" s="79"/>
-      <c r="N102" s="80">
+      <c r="M102" s="81"/>
+      <c r="N102" s="91">
         <f>L102-N101</f>
         <v>0</v>
       </c>
-      <c r="O102" s="80"/>
-      <c r="P102" s="77">
+      <c r="O102" s="91"/>
+      <c r="P102" s="89">
         <f>N102-P101</f>
         <v>0</v>
       </c>
-      <c r="Q102" s="78">
+      <c r="Q102" s="90">
         <f t="shared" ref="Q102:Y102" si="6">P102-Q101</f>
         <v>0</v>
       </c>
-      <c r="R102" s="79">
+      <c r="R102" s="81">
         <f>P102-R101</f>
         <v>0</v>
       </c>
-      <c r="S102" s="79">
+      <c r="S102" s="81">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T102" s="80">
+      <c r="T102" s="91">
         <f>R102-T101</f>
         <v>0</v>
       </c>
-      <c r="U102" s="80">
+      <c r="U102" s="91">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V102" s="77">
+      <c r="V102" s="89">
         <f>T102-V101</f>
         <v>0</v>
       </c>
-      <c r="W102" s="78">
+      <c r="W102" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X102" s="79">
+      <c r="X102" s="81">
         <f>V102-X101</f>
         <v>0</v>
       </c>
-      <c r="Y102" s="79">
+      <c r="Y102" s="81">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z102" s="79">
+      <c r="Z102" s="81">
         <f>X102-Z101</f>
         <v>0</v>
       </c>
-      <c r="AA102" s="79"/>
-      <c r="AB102" s="77">
+      <c r="AA102" s="81"/>
+      <c r="AB102" s="89">
         <f>Z102-AB101</f>
         <v>0</v>
       </c>
-      <c r="AC102" s="77"/>
+      <c r="AC102" s="89"/>
     </row>
     <row r="103" spans="1:29" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B103" s="29" t="s">
@@ -11154,79 +11158,79 @@
       </c>
       <c r="K103" s="62">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L103" s="56">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M103" s="56">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N103" s="61">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O103" s="61">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="P103" s="49">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="Q103" s="62">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="R103" s="56">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S103" s="56">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="T103" s="61">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="U103" s="61">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="V103" s="49">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="W103" s="62">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="X103" s="56">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="Y103" s="56">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="Z103" s="61">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AA103" s="61">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AB103" s="49">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AC103" s="49">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:29" s="26" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -11239,68 +11243,68 @@
       </c>
       <c r="E104" s="44">
         <f>SUM(F100:AC100)</f>
-        <v>0</v>
-      </c>
-      <c r="F104" s="86">
+        <v>4</v>
+      </c>
+      <c r="F104" s="88">
         <f>(F100+G100)</f>
         <v>0</v>
       </c>
-      <c r="G104" s="86"/>
-      <c r="H104" s="86">
+      <c r="G104" s="88"/>
+      <c r="H104" s="88">
         <f>(H100+I100)</f>
         <v>0</v>
       </c>
-      <c r="I104" s="86"/>
-      <c r="J104" s="86">
+      <c r="I104" s="88"/>
+      <c r="J104" s="88">
         <f>(J100+K100)</f>
-        <v>0</v>
-      </c>
-      <c r="K104" s="86"/>
-      <c r="L104" s="86">
+        <v>4</v>
+      </c>
+      <c r="K104" s="88"/>
+      <c r="L104" s="88">
         <f>(L100+M100)</f>
         <v>0</v>
       </c>
-      <c r="M104" s="86"/>
-      <c r="N104" s="86">
+      <c r="M104" s="88"/>
+      <c r="N104" s="88">
         <f>(N100+O100)</f>
         <v>0</v>
       </c>
-      <c r="O104" s="86"/>
-      <c r="P104" s="86">
+      <c r="O104" s="88"/>
+      <c r="P104" s="88">
         <f>(P100+Q100)</f>
         <v>0</v>
       </c>
-      <c r="Q104" s="86"/>
-      <c r="R104" s="86">
+      <c r="Q104" s="88"/>
+      <c r="R104" s="88">
         <f>(R100+S100)</f>
         <v>0</v>
       </c>
-      <c r="S104" s="86"/>
-      <c r="T104" s="86">
+      <c r="S104" s="88"/>
+      <c r="T104" s="88">
         <f>(T100+U100)</f>
         <v>0</v>
       </c>
-      <c r="U104" s="86"/>
-      <c r="V104" s="86">
+      <c r="U104" s="88"/>
+      <c r="V104" s="88">
         <f>(V100+W100)</f>
         <v>0</v>
       </c>
-      <c r="W104" s="86"/>
-      <c r="X104" s="86">
+      <c r="W104" s="88"/>
+      <c r="X104" s="88">
         <f>(X100+Y100)</f>
         <v>0</v>
       </c>
-      <c r="Y104" s="86"/>
-      <c r="Z104" s="86">
+      <c r="Y104" s="88"/>
+      <c r="Z104" s="88">
         <f>(Z100+AA100)</f>
         <v>0</v>
       </c>
-      <c r="AA104" s="86"/>
-      <c r="AB104" s="86">
+      <c r="AA104" s="88"/>
+      <c r="AB104" s="88">
         <f>(AB100+AC100)</f>
         <v>0</v>
       </c>
-      <c r="AC104" s="86"/>
+      <c r="AC104" s="88"/>
     </row>
     <row r="105" spans="1:29" s="26" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B105" s="29" t="s">
@@ -11313,66 +11317,66 @@
       <c r="E105" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F105" s="88">
+      <c r="F105" s="82">
         <f>IF( F100+G100&gt;0, F100+G100/1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G105" s="88"/>
-      <c r="H105" s="87">
+      <c r="G105" s="82"/>
+      <c r="H105" s="80">
         <f>IF(H104&gt;0,(F104+H104)/2,0)</f>
         <v>0</v>
       </c>
-      <c r="I105" s="87"/>
-      <c r="J105" s="85">
+      <c r="I105" s="80"/>
+      <c r="J105" s="83">
         <f>IF(J104&gt;0,(F104+H104+J104)/3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="K105" s="89"/>
-      <c r="L105" s="88">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="K105" s="84"/>
+      <c r="L105" s="82">
         <f>IF(L104&gt;0,(F104+ H104+J104+L104)/4,0)</f>
         <v>0</v>
       </c>
-      <c r="M105" s="88"/>
-      <c r="N105" s="87">
+      <c r="M105" s="82"/>
+      <c r="N105" s="80">
         <f>IF(N104&gt;0,(F104+H104 +J104+L104+N104)/5,0)</f>
         <v>0</v>
       </c>
-      <c r="O105" s="87"/>
-      <c r="P105" s="85">
+      <c r="O105" s="80"/>
+      <c r="P105" s="83">
         <f>IF(P104&gt;0,(F104+H104+J104 +L104+N104+P104)/6,0)</f>
         <v>0</v>
       </c>
-      <c r="Q105" s="89"/>
-      <c r="R105" s="88">
+      <c r="Q105" s="84"/>
+      <c r="R105" s="82">
         <f>IF(R104&gt;0,(F104+H104+J104+L104 +N104+P104+R104)/7,0)</f>
         <v>0</v>
       </c>
-      <c r="S105" s="88"/>
-      <c r="T105" s="87">
+      <c r="S105" s="82"/>
+      <c r="T105" s="80">
         <f>IF(T104&gt;0,(F104+H104+J104+L104+N104+ P104+R104+T104)/8,0)</f>
         <v>0</v>
       </c>
-      <c r="U105" s="87"/>
-      <c r="V105" s="85">
+      <c r="U105" s="80"/>
+      <c r="V105" s="83">
         <f>IF(V104&gt;0,(F104+H104+J104+L104+N104+P104+ R104+T104+V104)/9,0)</f>
         <v>0</v>
       </c>
-      <c r="W105" s="89"/>
-      <c r="X105" s="88">
+      <c r="W105" s="84"/>
+      <c r="X105" s="82">
         <f>IF(X104&gt;0,(F104+H104+J104+L104+N104+P104+R104 +T104+V104+X104)/10,0)</f>
         <v>0</v>
       </c>
-      <c r="Y105" s="88"/>
-      <c r="Z105" s="87">
+      <c r="Y105" s="82"/>
+      <c r="Z105" s="80">
         <f>IF(Z104&gt;0,(F104+H104+J104+L104+N104+P104+R104+ T104+V104+X104+Z104)/11,0)</f>
         <v>0</v>
       </c>
-      <c r="AA105" s="87"/>
-      <c r="AB105" s="85">
+      <c r="AA105" s="80"/>
+      <c r="AB105" s="83">
         <f>IF(AB104&gt;0,(F104+H104+J104+L104+N104+P104+R104+T104+V104+X104+Z104)/12,0)</f>
         <v>0</v>
       </c>
-      <c r="AC105" s="85"/>
+      <c r="AC105" s="83"/>
     </row>
     <row r="106" spans="1:29" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="107" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11444,19 +11448,42 @@
     <row r="173" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="Z105:AA105"/>
-    <mergeCell ref="Z102:AA102"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="L105:M105"/>
-    <mergeCell ref="N105:O105"/>
-    <mergeCell ref="P105:Q105"/>
-    <mergeCell ref="R105:S105"/>
-    <mergeCell ref="T105:U105"/>
-    <mergeCell ref="V105:W105"/>
-    <mergeCell ref="X105:Y105"/>
-    <mergeCell ref="X102:Y102"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="P102:Q102"/>
+    <mergeCell ref="R102:S102"/>
+    <mergeCell ref="T102:U102"/>
+    <mergeCell ref="V102:W102"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="AB102:AC102"/>
+    <mergeCell ref="P101:Q101"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="R101:S101"/>
+    <mergeCell ref="T101:U101"/>
+    <mergeCell ref="V101:W101"/>
+    <mergeCell ref="X101:Y101"/>
+    <mergeCell ref="AB101:AC101"/>
+    <mergeCell ref="Z101:AA101"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
@@ -11473,42 +11500,19 @@
     <mergeCell ref="X104:Y104"/>
     <mergeCell ref="AB104:AC104"/>
     <mergeCell ref="Z104:AA104"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="AB102:AC102"/>
-    <mergeCell ref="P101:Q101"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="R101:S101"/>
-    <mergeCell ref="T101:U101"/>
-    <mergeCell ref="V101:W101"/>
-    <mergeCell ref="X101:Y101"/>
-    <mergeCell ref="AB101:AC101"/>
-    <mergeCell ref="Z101:AA101"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="P102:Q102"/>
-    <mergeCell ref="R102:S102"/>
-    <mergeCell ref="T102:U102"/>
-    <mergeCell ref="V102:W102"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="L102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="Z105:AA105"/>
+    <mergeCell ref="Z102:AA102"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="L105:M105"/>
+    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="P105:Q105"/>
+    <mergeCell ref="R105:S105"/>
+    <mergeCell ref="T105:U105"/>
+    <mergeCell ref="V105:W105"/>
+    <mergeCell ref="X105:Y105"/>
+    <mergeCell ref="X102:Y102"/>
   </mergeCells>
   <conditionalFormatting sqref="B103:I103 B102:F102 H102">
     <cfRule type="cellIs" dxfId="46" priority="70" operator="lessThan">
@@ -11780,7 +11784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajustes y limpia archivos
</commit_message>
<xml_diff>
--- a/Plan/Proyectos Operaciones DCTI 2018(SCRUM).xlsx
+++ b/Plan/Proyectos Operaciones DCTI 2018(SCRUM).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG + STORIES" sheetId="2" r:id="rId1"/>
@@ -1077,25 +1077,19 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="16" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="23" fillId="15" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="14" borderId="12" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="15" fillId="14" borderId="15" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
@@ -1104,19 +1098,25 @@
     <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="14" borderId="12" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="16" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="12" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="23" fillId="15" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="17" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="14" borderId="15" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1737,7 +1737,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1925,9 +1924,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1997,7 +1994,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2221,7 +2217,7 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>16</c:v>
@@ -2347,7 +2343,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2479,7 +2474,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2552,7 +2546,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2671,7 +2664,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2847,10 +2839,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6666666666666665</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3075,7 +3067,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3371,7 +3362,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6105,9 +6095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5:G12"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -7264,11 +7254,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7300,77 +7290,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="88"/>
-      <c r="H1" s="86" t="s">
+      <c r="G1" s="86"/>
+      <c r="H1" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="87" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="88" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="86" t="s">
+      <c r="M1" s="86"/>
+      <c r="N1" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="86"/>
-      <c r="P1" s="87" t="s">
+      <c r="O1" s="87"/>
+      <c r="P1" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88" t="s">
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="88"/>
-      <c r="T1" s="86" t="s">
+      <c r="S1" s="86"/>
+      <c r="T1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="86"/>
-      <c r="V1" s="87" t="s">
+      <c r="U1" s="87"/>
+      <c r="V1" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="87"/>
-      <c r="X1" s="88" t="s">
+      <c r="W1" s="85"/>
+      <c r="X1" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="86" t="s">
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="87" t="s">
+      <c r="AA1" s="87"/>
+      <c r="AB1" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="87"/>
+      <c r="AC1" s="85"/>
       <c r="AD1" s="43"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="50">
         <v>1</v>
       </c>
@@ -7499,11 +7489,9 @@
       <c r="I4" s="59"/>
       <c r="J4" s="47"/>
       <c r="K4" s="63">
-        <v>6</v>
-      </c>
-      <c r="L4" s="53">
-        <v>4</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="L4" s="53"/>
       <c r="M4" s="53"/>
       <c r="N4" s="60"/>
       <c r="O4" s="59"/>
@@ -10926,11 +10914,11 @@
       </c>
       <c r="K100" s="65">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L100" s="56">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M100" s="56">
         <f t="shared" si="4"/>
@@ -11011,32 +10999,32 @@
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="12"/>
-      <c r="F101" s="85"/>
-      <c r="G101" s="83"/>
-      <c r="H101" s="84"/>
-      <c r="I101" s="84"/>
-      <c r="J101" s="81">
+      <c r="F101" s="93"/>
+      <c r="G101" s="81"/>
+      <c r="H101" s="91"/>
+      <c r="I101" s="91"/>
+      <c r="J101" s="89">
         <v>28</v>
       </c>
-      <c r="K101" s="82"/>
-      <c r="L101" s="83"/>
-      <c r="M101" s="83"/>
-      <c r="N101" s="84"/>
-      <c r="O101" s="84"/>
-      <c r="P101" s="81"/>
-      <c r="Q101" s="82"/>
-      <c r="R101" s="83"/>
-      <c r="S101" s="83"/>
-      <c r="T101" s="84"/>
-      <c r="U101" s="84"/>
-      <c r="V101" s="81"/>
-      <c r="W101" s="82"/>
-      <c r="X101" s="83"/>
-      <c r="Y101" s="83"/>
-      <c r="Z101" s="84"/>
-      <c r="AA101" s="84"/>
-      <c r="AB101" s="81"/>
-      <c r="AC101" s="81"/>
+      <c r="K101" s="90"/>
+      <c r="L101" s="81"/>
+      <c r="M101" s="81"/>
+      <c r="N101" s="91"/>
+      <c r="O101" s="91"/>
+      <c r="P101" s="89"/>
+      <c r="Q101" s="90"/>
+      <c r="R101" s="81"/>
+      <c r="S101" s="81"/>
+      <c r="T101" s="91"/>
+      <c r="U101" s="91"/>
+      <c r="V101" s="89"/>
+      <c r="W101" s="90"/>
+      <c r="X101" s="81"/>
+      <c r="Y101" s="81"/>
+      <c r="Z101" s="91"/>
+      <c r="AA101" s="91"/>
+      <c r="AB101" s="89"/>
+      <c r="AC101" s="89"/>
     </row>
     <row r="102" spans="1:29" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B102" s="29" t="s">
@@ -11050,81 +11038,81 @@
         <f>C100</f>
         <v>28</v>
       </c>
-      <c r="F102" s="83">
+      <c r="F102" s="81">
         <f>E102-F101</f>
         <v>28</v>
       </c>
-      <c r="G102" s="83"/>
-      <c r="H102" s="84">
+      <c r="G102" s="81"/>
+      <c r="H102" s="91">
         <f>F102-H101</f>
         <v>28</v>
       </c>
-      <c r="I102" s="84"/>
-      <c r="J102" s="81">
+      <c r="I102" s="91"/>
+      <c r="J102" s="89">
         <f>H102-J101</f>
         <v>0</v>
       </c>
-      <c r="K102" s="82"/>
-      <c r="L102" s="83">
+      <c r="K102" s="90"/>
+      <c r="L102" s="81">
         <f>J102-L101</f>
         <v>0</v>
       </c>
-      <c r="M102" s="83"/>
-      <c r="N102" s="84">
+      <c r="M102" s="81"/>
+      <c r="N102" s="91">
         <f>L102-N101</f>
         <v>0</v>
       </c>
-      <c r="O102" s="84"/>
-      <c r="P102" s="81">
+      <c r="O102" s="91"/>
+      <c r="P102" s="89">
         <f>N102-P101</f>
         <v>0</v>
       </c>
-      <c r="Q102" s="82">
+      <c r="Q102" s="90">
         <f t="shared" ref="Q102:Y102" si="6">P102-Q101</f>
         <v>0</v>
       </c>
-      <c r="R102" s="83">
+      <c r="R102" s="81">
         <f>P102-R101</f>
         <v>0</v>
       </c>
-      <c r="S102" s="83">
+      <c r="S102" s="81">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T102" s="84">
+      <c r="T102" s="91">
         <f>R102-T101</f>
         <v>0</v>
       </c>
-      <c r="U102" s="84">
+      <c r="U102" s="91">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V102" s="81">
+      <c r="V102" s="89">
         <f>T102-V101</f>
         <v>0</v>
       </c>
-      <c r="W102" s="82">
+      <c r="W102" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X102" s="83">
+      <c r="X102" s="81">
         <f>V102-X101</f>
         <v>0</v>
       </c>
-      <c r="Y102" s="83">
+      <c r="Y102" s="81">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z102" s="83">
+      <c r="Z102" s="81">
         <f>X102-Z101</f>
         <v>0</v>
       </c>
-      <c r="AA102" s="83"/>
-      <c r="AB102" s="81">
+      <c r="AA102" s="81"/>
+      <c r="AB102" s="89">
         <f>Z102-AB101</f>
         <v>0</v>
       </c>
-      <c r="AC102" s="81"/>
+      <c r="AC102" s="89"/>
     </row>
     <row r="103" spans="1:29" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B103" s="29" t="s">
@@ -11160,7 +11148,7 @@
       </c>
       <c r="K103" s="62">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L103" s="56">
         <f t="shared" si="7"/>
@@ -11247,66 +11235,66 @@
         <f>SUM(F100:AC100)</f>
         <v>12</v>
       </c>
-      <c r="F104" s="90">
+      <c r="F104" s="88">
         <f>(F100+G100)</f>
         <v>0</v>
       </c>
-      <c r="G104" s="90"/>
-      <c r="H104" s="90">
+      <c r="G104" s="88"/>
+      <c r="H104" s="88">
         <f>(H100+I100)</f>
         <v>0</v>
       </c>
-      <c r="I104" s="90"/>
-      <c r="J104" s="90">
+      <c r="I104" s="88"/>
+      <c r="J104" s="88">
         <f>(J100+K100)</f>
-        <v>8</v>
-      </c>
-      <c r="K104" s="90"/>
-      <c r="L104" s="90">
+        <v>12</v>
+      </c>
+      <c r="K104" s="88"/>
+      <c r="L104" s="88">
         <f>(L100+M100)</f>
-        <v>4</v>
-      </c>
-      <c r="M104" s="90"/>
-      <c r="N104" s="90">
+        <v>0</v>
+      </c>
+      <c r="M104" s="88"/>
+      <c r="N104" s="88">
         <f>(N100+O100)</f>
         <v>0</v>
       </c>
-      <c r="O104" s="90"/>
-      <c r="P104" s="90">
+      <c r="O104" s="88"/>
+      <c r="P104" s="88">
         <f>(P100+Q100)</f>
         <v>0</v>
       </c>
-      <c r="Q104" s="90"/>
-      <c r="R104" s="90">
+      <c r="Q104" s="88"/>
+      <c r="R104" s="88">
         <f>(R100+S100)</f>
         <v>0</v>
       </c>
-      <c r="S104" s="90"/>
-      <c r="T104" s="90">
+      <c r="S104" s="88"/>
+      <c r="T104" s="88">
         <f>(T100+U100)</f>
         <v>0</v>
       </c>
-      <c r="U104" s="90"/>
-      <c r="V104" s="90">
+      <c r="U104" s="88"/>
+      <c r="V104" s="88">
         <f>(V100+W100)</f>
         <v>0</v>
       </c>
-      <c r="W104" s="90"/>
-      <c r="X104" s="90">
+      <c r="W104" s="88"/>
+      <c r="X104" s="88">
         <f>(X100+Y100)</f>
         <v>0</v>
       </c>
-      <c r="Y104" s="90"/>
-      <c r="Z104" s="90">
+      <c r="Y104" s="88"/>
+      <c r="Z104" s="88">
         <f>(Z100+AA100)</f>
         <v>0</v>
       </c>
-      <c r="AA104" s="90"/>
-      <c r="AB104" s="90">
+      <c r="AA104" s="88"/>
+      <c r="AB104" s="88">
         <f>(AB100+AC100)</f>
         <v>0</v>
       </c>
-      <c r="AC104" s="90"/>
+      <c r="AC104" s="88"/>
     </row>
     <row r="105" spans="1:29" s="26" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B105" s="29" t="s">
@@ -11319,66 +11307,66 @@
       <c r="E105" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F105" s="92">
+      <c r="F105" s="82">
         <f>IF( F100+G100&gt;0, F100+G100/1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G105" s="92"/>
-      <c r="H105" s="91">
+      <c r="G105" s="82"/>
+      <c r="H105" s="80">
         <f>IF(H104&gt;0,(F104+H104)/2,0)</f>
         <v>0</v>
       </c>
-      <c r="I105" s="91"/>
-      <c r="J105" s="89">
+      <c r="I105" s="80"/>
+      <c r="J105" s="83">
         <f>IF(J104&gt;0,(F104+H104+J104)/3,0)</f>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="K105" s="93"/>
-      <c r="L105" s="92">
+        <v>4</v>
+      </c>
+      <c r="K105" s="84"/>
+      <c r="L105" s="82">
         <f>IF(L104&gt;0,(F104+ H104+J104+L104)/4,0)</f>
-        <v>3</v>
-      </c>
-      <c r="M105" s="92"/>
-      <c r="N105" s="91">
+        <v>0</v>
+      </c>
+      <c r="M105" s="82"/>
+      <c r="N105" s="80">
         <f>IF(N104&gt;0,(F104+H104 +J104+L104+N104)/5,0)</f>
         <v>0</v>
       </c>
-      <c r="O105" s="91"/>
-      <c r="P105" s="89">
+      <c r="O105" s="80"/>
+      <c r="P105" s="83">
         <f>IF(P104&gt;0,(F104+H104+J104 +L104+N104+P104)/6,0)</f>
         <v>0</v>
       </c>
-      <c r="Q105" s="93"/>
-      <c r="R105" s="92">
+      <c r="Q105" s="84"/>
+      <c r="R105" s="82">
         <f>IF(R104&gt;0,(F104+H104+J104+L104 +N104+P104+R104)/7,0)</f>
         <v>0</v>
       </c>
-      <c r="S105" s="92"/>
-      <c r="T105" s="91">
+      <c r="S105" s="82"/>
+      <c r="T105" s="80">
         <f>IF(T104&gt;0,(F104+H104+J104+L104+N104+ P104+R104+T104)/8,0)</f>
         <v>0</v>
       </c>
-      <c r="U105" s="91"/>
-      <c r="V105" s="89">
+      <c r="U105" s="80"/>
+      <c r="V105" s="83">
         <f>IF(V104&gt;0,(F104+H104+J104+L104+N104+P104+ R104+T104+V104)/9,0)</f>
         <v>0</v>
       </c>
-      <c r="W105" s="93"/>
-      <c r="X105" s="92">
+      <c r="W105" s="84"/>
+      <c r="X105" s="82">
         <f>IF(X104&gt;0,(F104+H104+J104+L104+N104+P104+R104 +T104+V104+X104)/10,0)</f>
         <v>0</v>
       </c>
-      <c r="Y105" s="92"/>
-      <c r="Z105" s="91">
+      <c r="Y105" s="82"/>
+      <c r="Z105" s="80">
         <f>IF(Z104&gt;0,(F104+H104+J104+L104+N104+P104+R104+ T104+V104+X104+Z104)/11,0)</f>
         <v>0</v>
       </c>
-      <c r="AA105" s="91"/>
-      <c r="AB105" s="89">
+      <c r="AA105" s="80"/>
+      <c r="AB105" s="83">
         <f>IF(AB104&gt;0,(F104+H104+J104+L104+N104+P104+R104+T104+V104+X104+Z104)/12,0)</f>
         <v>0</v>
       </c>
-      <c r="AC105" s="89"/>
+      <c r="AC105" s="83"/>
     </row>
     <row r="106" spans="1:29" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="107" spans="1:29" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11450,19 +11438,42 @@
     <row r="173" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="Z105:AA105"/>
-    <mergeCell ref="Z102:AA102"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="L105:M105"/>
-    <mergeCell ref="N105:O105"/>
-    <mergeCell ref="P105:Q105"/>
-    <mergeCell ref="R105:S105"/>
-    <mergeCell ref="T105:U105"/>
-    <mergeCell ref="V105:W105"/>
-    <mergeCell ref="X105:Y105"/>
-    <mergeCell ref="X102:Y102"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="P102:Q102"/>
+    <mergeCell ref="R102:S102"/>
+    <mergeCell ref="T102:U102"/>
+    <mergeCell ref="V102:W102"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="L102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="AB102:AC102"/>
+    <mergeCell ref="P101:Q101"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="R101:S101"/>
+    <mergeCell ref="T101:U101"/>
+    <mergeCell ref="V101:W101"/>
+    <mergeCell ref="X101:Y101"/>
+    <mergeCell ref="AB101:AC101"/>
+    <mergeCell ref="Z101:AA101"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
@@ -11479,42 +11490,19 @@
     <mergeCell ref="X104:Y104"/>
     <mergeCell ref="AB104:AC104"/>
     <mergeCell ref="Z104:AA104"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="AB102:AC102"/>
-    <mergeCell ref="P101:Q101"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="R101:S101"/>
-    <mergeCell ref="T101:U101"/>
-    <mergeCell ref="V101:W101"/>
-    <mergeCell ref="X101:Y101"/>
-    <mergeCell ref="AB101:AC101"/>
-    <mergeCell ref="Z101:AA101"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="P102:Q102"/>
-    <mergeCell ref="R102:S102"/>
-    <mergeCell ref="T102:U102"/>
-    <mergeCell ref="V102:W102"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="L102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="Z105:AA105"/>
+    <mergeCell ref="Z102:AA102"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="L105:M105"/>
+    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="P105:Q105"/>
+    <mergeCell ref="R105:S105"/>
+    <mergeCell ref="T105:U105"/>
+    <mergeCell ref="V105:W105"/>
+    <mergeCell ref="X105:Y105"/>
+    <mergeCell ref="X102:Y102"/>
   </mergeCells>
   <conditionalFormatting sqref="B103:I103 B102:F102 H102">
     <cfRule type="cellIs" dxfId="46" priority="70" operator="lessThan">

</xml_diff>